<commit_message>
calculated days between dates of first egg laying and date of data collection
</commit_message>
<xml_diff>
--- a/raw_data/cpb_tei_mass_data.xlsx
+++ b/raw_data/cpb_tei_mass_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joegunn/Desktop/Projects/active_projects/CPB_Phenotype/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48019333-079A-8C42-B501-AABDE697CC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3473457B-70B8-BF4D-8C68-C7F904EFEE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1280" yWindow="2000" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -560,8 +560,8 @@
   </sheetPr>
   <dimension ref="A1:K996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A407" workbookViewId="0">
+      <selection activeCell="K434" sqref="K434"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -905,7 +905,7 @@
         <v>133.80000000000001</v>
       </c>
       <c r="J10" s="5">
-        <v>45344</v>
+        <v>45345</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>16</v>
@@ -939,7 +939,7 @@
         <v>167.7</v>
       </c>
       <c r="J11" s="5">
-        <v>45344</v>
+        <v>45345</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>16</v>
@@ -1515,11 +1515,9 @@
       <c r="H28" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I28" s="8">
-        <v>133.6</v>
-      </c>
+      <c r="I28" s="8"/>
       <c r="J28" s="5">
-        <v>45376</v>
+        <v>45400</v>
       </c>
       <c r="K28" s="4" t="s">
         <v>16</v>
@@ -1551,11 +1549,9 @@
       <c r="H29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I29" s="8">
-        <v>114.9</v>
-      </c>
+      <c r="I29" s="8"/>
       <c r="J29" s="5">
-        <v>45376</v>
+        <v>45400</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>16</v>
@@ -11798,11 +11794,9 @@
       <c r="I326" s="4">
         <v>124.4</v>
       </c>
-      <c r="J326" s="5">
-        <v>45436</v>
-      </c>
+      <c r="J326" s="5"/>
       <c r="K326" s="4" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
     </row>
     <row r="327" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -11834,11 +11828,9 @@
       <c r="I327" s="4">
         <v>91.4</v>
       </c>
-      <c r="J327" s="5">
-        <v>45436</v>
-      </c>
+      <c r="J327" s="5"/>
       <c r="K327" s="4" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
     </row>
     <row r="328" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -12006,9 +11998,11 @@
       <c r="I332" s="8">
         <v>90.3</v>
       </c>
-      <c r="J332" s="9"/>
+      <c r="J332" s="5">
+        <v>45444</v>
+      </c>
       <c r="K332" s="4" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
     </row>
     <row r="333" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -12040,9 +12034,11 @@
       <c r="I333" s="8">
         <v>104.1</v>
       </c>
-      <c r="J333" s="9"/>
+      <c r="J333" s="5">
+        <v>45444</v>
+      </c>
       <c r="K333" s="4" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
     </row>
     <row r="334" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14966,9 +14962,11 @@
       <c r="I418" s="8">
         <v>92.2</v>
       </c>
-      <c r="J418" s="9"/>
+      <c r="J418" s="5">
+        <v>45477</v>
+      </c>
       <c r="K418" s="4" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
     </row>
     <row r="419" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15000,9 +14998,11 @@
       <c r="I419" s="8">
         <v>79.5</v>
       </c>
-      <c r="J419" s="9"/>
+      <c r="J419" s="5">
+        <v>45477</v>
+      </c>
       <c r="K419" s="4" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
     </row>
     <row r="420" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15450,11 +15450,9 @@
       <c r="I432" s="8">
         <v>107.9</v>
       </c>
-      <c r="J432" s="5">
-        <v>45459</v>
-      </c>
+      <c r="J432" s="5"/>
       <c r="K432" s="4" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
     </row>
     <row r="433" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15486,11 +15484,9 @@
       <c r="I433" s="8">
         <v>103.8</v>
       </c>
-      <c r="J433" s="5">
-        <v>45459</v>
-      </c>
+      <c r="J433" s="5"/>
       <c r="K433" s="4" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
     </row>
     <row r="434" spans="1:11" ht="16" x14ac:dyDescent="0.2">

</xml_diff>